<commit_message>
Create plot showing % of problems with optimal algorithms per decade
</commit_message>
<xml_diff>
--- a/Analysis/Plots/Best Space Algos/Best Space Pie.xlsx
+++ b/Analysis/Plots/Best Space Algos/Best Space Pie.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haydenrome/Dropbox (MIT)/5 - MEng/AlgoWiki Research/AlgoWiki/Analysis/Plots/Best Space Algos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88F1F3FB-5A06-A24E-89F3-EED0A6865453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0B2BF7-6A23-3B4C-A387-DD07AA521379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17900" yWindow="-17620" windowWidth="28040" windowHeight="17260" xr2:uid="{DA6B6C6E-4554-8E4D-AE66-89131F495CA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -730,7 +730,11 @@
                     </a:fld>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:t> (</a:t>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" b="0" baseline="0"/>
+                      <a:t>(</a:t>
                     </a:r>
                     <a:fld id="{0EF512EF-FD5A-D64D-8BF9-4C9202FDA8C8}" type="PERCENTAGE">
                       <a:rPr lang="en-US" b="0" baseline="0"/>
@@ -825,7 +829,11 @@
                     </a:fld>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:t> (</a:t>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" b="0" baseline="0"/>
+                      <a:t>(</a:t>
                     </a:r>
                     <a:fld id="{E4CEDFCB-1F5C-CE4A-94EB-DD0D248C4061}" type="PERCENTAGE">
                       <a:rPr lang="en-US" b="0" baseline="0"/>
@@ -1040,6 +1048,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
@@ -2117,7 +2132,7 @@
   <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update for Neil's presentation
</commit_message>
<xml_diff>
--- a/Analysis/Plots/Best Space Algos/Best Space Pie.xlsx
+++ b/Analysis/Plots/Best Space Algos/Best Space Pie.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haydenrome/Dropbox (MIT)/5 - MEng/AlgoWiki Research/AlgoWiki/Analysis/Plots/Best Space Algos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA0B2CC-736F-D842-8CE6-820B710A8713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D701344-B793-8641-92C1-1A484068E9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="-18420" windowWidth="28040" windowHeight="17260" activeTab="1" xr2:uid="{DA6B6C6E-4554-8E4D-AE66-89131F495CA4}"/>
+    <workbookView xWindow="19560" yWindow="-20380" windowWidth="30360" windowHeight="19520" activeTab="1" xr2:uid="{DA6B6C6E-4554-8E4D-AE66-89131F495CA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Best Space" sheetId="1" r:id="rId1"/>
-    <sheet name="Improves space or time or both" sheetId="2" r:id="rId2"/>
+    <sheet name="Algorithms that Improve" sheetId="2" r:id="rId2"/>
+    <sheet name="Problems that Improve" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Constant</t>
   </si>
@@ -46,9 +47,6 @@
   </si>
   <si>
     <t>Linear</t>
-  </si>
-  <si>
-    <t>Quasilinear</t>
   </si>
   <si>
     <t>Quadratic</t>
@@ -83,6 +81,12 @@
   <si>
     <t>Improves both</t>
   </si>
+  <si>
+    <t>n log n</t>
+  </si>
+  <si>
+    <t>Not including first algorithm paper as an improvement</t>
+  </si>
 </sst>
 </file>
 
@@ -97,12 +101,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBD9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA946C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,9 +133,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,12 +146,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFA946C"/>
+      <color rgb="FFFFBD9B"/>
+      <color rgb="FFD7714A"/>
+      <color rgb="FFC14625"/>
+      <color rgb="FFEC9973"/>
+      <color rgb="FFFFC0A0"/>
       <color rgb="FFD2390F"/>
       <color rgb="FFE9542E"/>
       <color rgb="FFF9946A"/>
-      <color rgb="FFFFBD9B"/>
       <color rgb="FFE7693E"/>
-      <color rgb="FFB90000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -253,7 +275,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFBD9B"/>
+                <a:srgbClr val="FFC0A0"/>
               </a:solidFill>
               <a:ln w="3175">
                 <a:solidFill>
@@ -293,7 +315,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="E7693E"/>
+                <a:srgbClr val="EC9973"/>
               </a:solidFill>
               <a:ln w="3175">
                 <a:solidFill>
@@ -333,7 +355,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="D2390F"/>
+                <a:srgbClr val="D7714A"/>
               </a:solidFill>
               <a:ln w="3175">
                 <a:solidFill>
@@ -353,7 +375,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="B90000"/>
+                <a:srgbClr val="C14625"/>
               </a:solidFill>
               <a:ln w="3175">
                 <a:solidFill>
@@ -498,104 +520,9 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.11347517730496454"/>
-                  <c:y val="-5.1829268292683035E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                    <a:spAutoFit/>
-                  </a:bodyPr>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:fld id="{7B973BC1-30DF-0647-95AB-0ED0786D8C42}" type="CATEGORYNAME">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr>
-                        <a:defRPr>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:t>[CATEGORY NAME]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t> </a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" b="0" baseline="0"/>
-                      <a:t>(</a:t>
-                    </a:r>
-                    <a:fld id="{30730F29-69BE-BE49-A9A7-590B77FD46BF}" type="PERCENTAGE">
-                      <a:rPr lang="en-US" b="0" baseline="0"/>
-                      <a:pPr>
-                        <a:defRPr>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:t>[PERCENTAGE]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" b="0" baseline="0"/>
-                      <a:t>)</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
+              <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-C882-5447-BBCA-DC3C6F059FD0}"/>
                 </c:ext>
@@ -605,8 +532,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.11955420466058764"/>
-                  <c:y val="-4.878048780487805E-2"/>
+                  <c:x val="-7.5184494153880455E-2"/>
+                  <c:y val="1.2195121951219513E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -708,104 +635,9 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-6.0790273556231005E-2"/>
-                  <c:y val="0"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                    <a:spAutoFit/>
-                  </a:bodyPr>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:fld id="{0702AB3F-6A76-6947-BCB9-CD8B83105B3C}" type="CATEGORYNAME">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr>
-                        <a:defRPr>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:t>[CATEGORY NAME]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t> </a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" b="0" baseline="0"/>
-                      <a:t>(</a:t>
-                    </a:r>
-                    <a:fld id="{0EF512EF-FD5A-D64D-8BF9-4C9202FDA8C8}" type="PERCENTAGE">
-                      <a:rPr lang="en-US" b="0" baseline="0"/>
-                      <a:pPr>
-                        <a:defRPr>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:t>[PERCENTAGE]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" b="0" baseline="0"/>
-                      <a:t>)</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
+              <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-C882-5447-BBCA-DC3C6F059FD0}"/>
                 </c:ext>
@@ -920,8 +752,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.22514329253719539"/>
-                  <c:y val="-1.2195121951219499E-2"/>
+                  <c:x val="0.20094161058382104"/>
+                  <c:y val="3.0487804878048643E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1137,7 +969,7 @@
                   <c:v>Linear</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Quasilinear</c:v>
+                  <c:v>n log n</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Polynomial</c:v>
@@ -1155,22 +987,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1280,11 +1112,27 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Percentage of Algorithms that Give Improvements</a:t>
+              <a:t>Percentage of Algorithm</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Papers</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> that Give Improvements (starting with the first paper)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13168562564632885"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1335,7 +1183,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFBD9B"/>
+                <a:srgbClr val="FFC0A0"/>
               </a:solidFill>
               <a:ln w="3175">
                 <a:solidFill>
@@ -1346,7 +1194,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-8A34-6B47-94A2-116F3C8C0869}"/>
+                <c16:uniqueId val="{00000001-1301-2341-9102-F953747FCA52}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1355,7 +1203,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="F9946A"/>
+                <a:srgbClr val="EC9973"/>
               </a:solidFill>
               <a:ln w="3175">
                 <a:solidFill>
@@ -1366,7 +1214,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-8A34-6B47-94A2-116F3C8C0869}"/>
+                <c16:uniqueId val="{00000003-1301-2341-9102-F953747FCA52}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1375,7 +1223,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="E9542E"/>
+                <a:srgbClr val="D7714A"/>
               </a:solidFill>
               <a:ln w="3175">
                 <a:solidFill>
@@ -1386,7 +1234,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-8A34-6B47-94A2-116F3C8C0869}"/>
+                <c16:uniqueId val="{00000005-1301-2341-9102-F953747FCA52}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1395,7 +1243,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="D2390F"/>
+                <a:srgbClr val="C14625"/>
               </a:solidFill>
               <a:ln w="3175">
                 <a:solidFill>
@@ -1406,7 +1254,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-8A34-6B47-94A2-116F3C8C0869}"/>
+                <c16:uniqueId val="{00000007-1301-2341-9102-F953747FCA52}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1415,8 +1263,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.13650465356772E-2"/>
-                  <c:y val="-6.0790273556231003E-3"/>
+                  <c:x val="9.927611168562564E-2"/>
+                  <c:y val="-0.10334346504559271"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1436,7 +1284,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{1107B058-E7A8-C94A-83AA-DF00B3F04995}" type="CATEGORYNAME">
+                    <a:fld id="{25E84737-0389-1D43-9D16-51244DAE4755}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr>
@@ -1455,7 +1303,7 @@
                       <a:rPr lang="en-US" b="0" baseline="0"/>
                       <a:t>(</a:t>
                     </a:r>
-                    <a:fld id="{4BE9D8DD-B34C-2F40-A541-F307C9008CB4}" type="VALUE">
+                    <a:fld id="{E4443BF7-111A-B343-810D-7B8F129E514A}" type="PERCENTAGE">
                       <a:rPr lang="en-US" b="0" baseline="0"/>
                       <a:pPr>
                         <a:defRPr>
@@ -1464,7 +1312,7 @@
                           </a:solidFill>
                         </a:defRPr>
                       </a:pPr>
-                      <a:t>[VALUE]</a:t>
+                      <a:t>[PERCENTAGE]</a:t>
                     </a:fld>
                     <a:r>
                       <a:rPr lang="en-US" b="0" baseline="0"/>
@@ -1501,10 +1349,10 @@
               </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
+              <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:separator> </c:separator>
               <c:extLst>
@@ -1513,7 +1361,7 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-8A34-6B47-94A2-116F3C8C0869}"/>
+                  <c16:uniqueId val="{00000001-1301-2341-9102-F953747FCA52}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1521,8 +1369,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.2047569803516028E-2"/>
-                  <c:y val="1.5197568389057751E-2"/>
+                  <c:x val="-0.10961737331954498"/>
+                  <c:y val="0.1063829787234042"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1542,7 +1390,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{B96EF10C-DEAE-C048-B0F4-5A098172F3C9}" type="CATEGORYNAME">
+                    <a:fld id="{27702CFB-133B-0D42-9F00-DCF0CC099F5C}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr>
@@ -1561,7 +1409,7 @@
                       <a:rPr lang="en-US" b="0" baseline="0"/>
                       <a:t>(</a:t>
                     </a:r>
-                    <a:fld id="{96A83574-58A5-774F-B711-4F3024AE0E62}" type="VALUE">
+                    <a:fld id="{E29DF9F7-352C-0A4D-AD2C-616FF569BAFE}" type="PERCENTAGE">
                       <a:rPr lang="en-US" b="0" baseline="0"/>
                       <a:pPr>
                         <a:defRPr>
@@ -1570,7 +1418,7 @@
                           </a:solidFill>
                         </a:defRPr>
                       </a:pPr>
-                      <a:t>[VALUE]</a:t>
+                      <a:t>[PERCENTAGE]</a:t>
                     </a:fld>
                     <a:r>
                       <a:rPr lang="en-US" b="0" baseline="0"/>
@@ -1607,10 +1455,10 @@
               </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
+              <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:separator> </c:separator>
               <c:extLst>
@@ -1619,7 +1467,7 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-8A34-6B47-94A2-116F3C8C0869}"/>
+                  <c16:uniqueId val="{00000003-1301-2341-9102-F953747FCA52}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1627,8 +1475,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.8252326783867626E-2"/>
-                  <c:y val="-6.0790273556231003E-3"/>
+                  <c:x val="-0.19027921406411583"/>
+                  <c:y val="3.590760844243579E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1648,7 +1496,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{F216B955-563B-5B41-A9D3-4D3558974059}" type="CATEGORYNAME">
+                    <a:fld id="{0921A842-B124-D743-8326-70DC28996C41}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr>
@@ -1667,7 +1515,7 @@
                       <a:rPr lang="en-US" b="0" baseline="0"/>
                       <a:t>(</a:t>
                     </a:r>
-                    <a:fld id="{4637A3E1-6C19-BC4A-9589-BAD4DDBBE460}" type="VALUE">
+                    <a:fld id="{1D802A81-4CA5-6C41-99BA-68E13CD775B6}" type="PERCENTAGE">
                       <a:rPr lang="en-US" b="0" baseline="0"/>
                       <a:pPr>
                         <a:defRPr>
@@ -1676,7 +1524,7 @@
                           </a:solidFill>
                         </a:defRPr>
                       </a:pPr>
-                      <a:t>[VALUE]</a:t>
+                      <a:t>[PERCENTAGE]</a:t>
                     </a:fld>
                     <a:r>
                       <a:rPr lang="en-US" b="0" baseline="0"/>
@@ -1713,10 +1561,10 @@
               </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
+              <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:separator> </c:separator>
               <c:extLst>
@@ -1725,7 +1573,7 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-8A34-6B47-94A2-116F3C8C0869}"/>
+                  <c16:uniqueId val="{00000005-1301-2341-9102-F953747FCA52}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1733,8 +1581,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.3092037228541892E-2"/>
-                  <c:y val="-2.4316109422492401E-2"/>
+                  <c:x val="0.22543950361944157"/>
+                  <c:y val="-1.1996226063458045E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1754,7 +1602,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{C848C495-A87E-2848-A828-8D2804B9967D}" type="CATEGORYNAME">
+                    <a:fld id="{59CC0F4E-977C-EE49-8142-FD529B2AE645}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr>
@@ -1773,7 +1621,7 @@
                       <a:rPr lang="en-US" b="0" baseline="0"/>
                       <a:t>(</a:t>
                     </a:r>
-                    <a:fld id="{49AF9A3E-0F01-C94F-90B3-BB018A5BE2FF}" type="VALUE">
+                    <a:fld id="{1420EBB9-A22B-2C4E-9268-9478C933DE67}" type="PERCENTAGE">
                       <a:rPr lang="en-US" b="0" baseline="0"/>
                       <a:pPr>
                         <a:defRPr>
@@ -1782,7 +1630,7 @@
                           </a:solidFill>
                         </a:defRPr>
                       </a:pPr>
-                      <a:t>[VALUE]</a:t>
+                      <a:t>[PERCENTAGE]</a:t>
                     </a:fld>
                     <a:r>
                       <a:rPr lang="en-US" b="0" baseline="0"/>
@@ -1819,10 +1667,10 @@
               </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
+              <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:separator> </c:separator>
               <c:extLst>
@@ -1831,12 +1679,16 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-8A34-6B47-94A2-116F3C8C0869}"/>
+                  <c16:uniqueId val="{00000007-1301-2341-9102-F953747FCA52}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
               <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
             </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -1859,22 +1711,21 @@
             </c:txPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
+            <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:separator> </c:separator>
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
               <c:spPr>
-                <a:ln w="3175" cap="sq" cmpd="sng" algn="ctr">
+                <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
-                  <a:miter lim="800000"/>
+                  <a:round/>
                   <a:headEnd type="oval" w="sm" len="sm"/>
-                  <a:tailEnd type="none" w="sm" len="sm"/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
@@ -1885,7 +1736,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Improves space or time or both'!$B$4:$B$7</c:f>
+              <c:f>'Algorithms that Improve'!$B$10:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1905,28 +1756,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Improves space or time or both'!$C$4:$C$7</c:f>
+              <c:f>'Algorithms that Improve'!$C$10:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8A34-6B47-94A2-116F3C8C0869}"/>
+              <c16:uniqueId val="{00000008-1301-2341-9102-F953747FCA52}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3159,27 +3010,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3761182-628E-80D2-8499-9CF5C0F0C720}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B53F3EF9-00C9-3049-AA6D-5B4AD53D6FF4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3496,17 +3349,17 @@
   <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
@@ -3514,7 +3367,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -3522,7 +3375,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -3530,52 +3383,52 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <f>SUM(E7:E9)</f>
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3586,10 +3439,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C790AD49-AC62-314E-9F95-122ED9179127}">
-  <dimension ref="B4:C7"/>
+  <dimension ref="B4:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3598,39 +3451,129 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.55000000000000004</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.13</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.03</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.28000000000000003</v>
-      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF1EA56-A6D8-E243-9DF9-7D3953B924FA}">
+  <dimension ref="B4:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>